<commit_message>
feat: add functions to compute power from torque and rotation rate
Add functions to compute power from torque and rotation rate. Output power in units of lbf-ft/sec, horsepower, watts and kilowatts. Input torque in lbf-ft, lbf-in and N-m. Input rotation rate in rev/min and rev/sec.
</commit_message>
<xml_diff>
--- a/Reference/AeroToolKitFunctionList.xlsx
+++ b/Reference/AeroToolKitFunctionList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fs272\AeroProgs\StdAtmoAddIn\AeroToolKitAddIn\Reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB7748A-BE67-4223-BCBE-C1C91922509C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85BD5A6-22D0-4BF7-B1A0-DC7042AF1405}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AeroToolKitFunctionList" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2786" uniqueCount="979">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2882" uniqueCount="1016">
   <si>
     <t>KCAS</t>
   </si>
@@ -2983,6 +2983,117 @@
   </si>
   <si>
     <t>metric ton ("tonne")</t>
+  </si>
+  <si>
+    <t>AeroPower_ftLbfPerSec_fTorqueLbfFtRevPerMin</t>
+  </si>
+  <si>
+    <t>AeroPower_ftLbfPerSec_fTorqueLbfFtRevPerSec</t>
+  </si>
+  <si>
+    <t>AeroPower_ftLbfPerSec_fTorqueLbfInchRevPerMin</t>
+  </si>
+  <si>
+    <t>AeroPower_ftLbfPerSec_fTorqueLbfInchRevPerSec</t>
+  </si>
+  <si>
+    <t>AeroPower_horsepower_fTorqueLbfFtRevPerMin</t>
+  </si>
+  <si>
+    <t>AeroPower_horsepower_fTorqueLbfFtRevPerSec</t>
+  </si>
+  <si>
+    <t>AeroPower_horsepower_fTorqueLbfInchRevPerMin</t>
+  </si>
+  <si>
+    <t>AeroPower_horsepower_fTorqueLbfInchRevPerSec</t>
+  </si>
+  <si>
+    <t>AeroPower_watts_fTorqueNewtonMeterRevPerMin</t>
+  </si>
+  <si>
+    <t>AeroPower_watts_fTorqueNewtonMeterRevPerSec</t>
+  </si>
+  <si>
+    <t>AeroPower_kilowatts_fTorqueNewtonMeterRevPerMin</t>
+  </si>
+  <si>
+    <t>AeroPower_kilowatts_fTorqueNewtonMeterRevPerSec</t>
+  </si>
+  <si>
+    <t>torqueLbfFt</t>
+  </si>
+  <si>
+    <t>revPerMin</t>
+  </si>
+  <si>
+    <t>revPerSec</t>
+  </si>
+  <si>
+    <t>torqueLbfInch</t>
+  </si>
+  <si>
+    <t>newtonMeter</t>
+  </si>
+  <si>
+    <t>lbf-ft/sec</t>
+  </si>
+  <si>
+    <t>watts</t>
+  </si>
+  <si>
+    <t>kilowatts</t>
+  </si>
+  <si>
+    <t>lbf-ft/sec, f(torque in lbf-ft, RPM)</t>
+  </si>
+  <si>
+    <t>lbf-ft/sec, f(torque in lbf-ft, RPS)</t>
+  </si>
+  <si>
+    <t>lbf-ft/sec, f(torque in lbf-inch, RPM)</t>
+  </si>
+  <si>
+    <t>lbf-ft/sec, f(torque in lbf-inch, RPS)</t>
+  </si>
+  <si>
+    <t>horsepower, f(torque in lbf-ft, RPS)</t>
+  </si>
+  <si>
+    <t>horsepower, f(torque in lbf-inch, RPM)</t>
+  </si>
+  <si>
+    <t>horsepower, f(torque in lbf-inch, RPS)</t>
+  </si>
+  <si>
+    <t>watts, f(torque in newton-meter, RPM)</t>
+  </si>
+  <si>
+    <t>watts, f(torque in newton-meter, RPS)</t>
+  </si>
+  <si>
+    <t>kilowatts, f(torque in newton-meter, RPM)</t>
+  </si>
+  <si>
+    <t>kilowatts, f(torque in newton-meter, RPS)</t>
+  </si>
+  <si>
+    <t>lbf-ft, RPM</t>
+  </si>
+  <si>
+    <t>lbf-ft, RPS</t>
+  </si>
+  <si>
+    <t>lbf-inch, RPM</t>
+  </si>
+  <si>
+    <t>lbf-inch, RPS</t>
+  </si>
+  <si>
+    <t>newton-meter, RPM</t>
+  </si>
+  <si>
+    <t>newton-meter, RPS</t>
   </si>
 </sst>
 </file>
@@ -3224,7 +3335,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3265,6 +3376,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -3674,17 +3786,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K365"/>
+  <dimension ref="A1:K377"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -13868,6 +13978,354 @@
       </c>
       <c r="K365" s="2" t="s">
         <v>602</v>
+      </c>
+    </row>
+    <row r="366" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A366" s="34" t="s">
+        <v>855</v>
+      </c>
+      <c r="B366" s="32" t="s">
+        <v>855</v>
+      </c>
+      <c r="C366" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="D366" s="2" t="s">
+        <v>991</v>
+      </c>
+      <c r="E366" s="2" t="s">
+        <v>992</v>
+      </c>
+      <c r="H366" s="2">
+        <v>2</v>
+      </c>
+      <c r="I366" t="s">
+        <v>999</v>
+      </c>
+      <c r="J366" t="s">
+        <v>1010</v>
+      </c>
+      <c r="K366" s="2" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="367" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A367" s="34" t="s">
+        <v>855</v>
+      </c>
+      <c r="B367" s="32" t="s">
+        <v>855</v>
+      </c>
+      <c r="C367" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="D367" s="2" t="s">
+        <v>991</v>
+      </c>
+      <c r="E367" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="H367" s="2">
+        <v>2</v>
+      </c>
+      <c r="I367" t="s">
+        <v>1000</v>
+      </c>
+      <c r="J367" t="s">
+        <v>1011</v>
+      </c>
+      <c r="K367" s="2" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="368" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A368" s="34" t="s">
+        <v>855</v>
+      </c>
+      <c r="B368" s="32" t="s">
+        <v>855</v>
+      </c>
+      <c r="C368" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="D368" s="2" t="s">
+        <v>994</v>
+      </c>
+      <c r="E368" s="2" t="s">
+        <v>992</v>
+      </c>
+      <c r="H368" s="2">
+        <v>2</v>
+      </c>
+      <c r="I368" t="s">
+        <v>1001</v>
+      </c>
+      <c r="J368" t="s">
+        <v>1012</v>
+      </c>
+      <c r="K368" s="2" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="369" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A369" s="34" t="s">
+        <v>855</v>
+      </c>
+      <c r="B369" s="32" t="s">
+        <v>855</v>
+      </c>
+      <c r="C369" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="D369" s="2" t="s">
+        <v>994</v>
+      </c>
+      <c r="E369" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="H369" s="2">
+        <v>2</v>
+      </c>
+      <c r="I369" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J369" t="s">
+        <v>1013</v>
+      </c>
+      <c r="K369" s="2" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="370" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A370" s="34" t="s">
+        <v>855</v>
+      </c>
+      <c r="B370" s="32" t="s">
+        <v>855</v>
+      </c>
+      <c r="C370" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="D370" s="2" t="s">
+        <v>991</v>
+      </c>
+      <c r="E370" s="2" t="s">
+        <v>992</v>
+      </c>
+      <c r="H370" s="2">
+        <v>2</v>
+      </c>
+      <c r="I370" t="s">
+        <v>999</v>
+      </c>
+      <c r="J370" t="s">
+        <v>1010</v>
+      </c>
+      <c r="K370" s="2" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="371" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A371" s="34" t="s">
+        <v>855</v>
+      </c>
+      <c r="B371" s="32" t="s">
+        <v>855</v>
+      </c>
+      <c r="C371" s="3" t="s">
+        <v>984</v>
+      </c>
+      <c r="D371" s="2" t="s">
+        <v>991</v>
+      </c>
+      <c r="E371" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="H371" s="2">
+        <v>2</v>
+      </c>
+      <c r="I371" t="s">
+        <v>1003</v>
+      </c>
+      <c r="J371" t="s">
+        <v>1011</v>
+      </c>
+      <c r="K371" s="2" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="372" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A372" s="34" t="s">
+        <v>855</v>
+      </c>
+      <c r="B372" s="32" t="s">
+        <v>855</v>
+      </c>
+      <c r="C372" s="3" t="s">
+        <v>985</v>
+      </c>
+      <c r="D372" s="2" t="s">
+        <v>994</v>
+      </c>
+      <c r="E372" s="2" t="s">
+        <v>992</v>
+      </c>
+      <c r="H372" s="2">
+        <v>2</v>
+      </c>
+      <c r="I372" t="s">
+        <v>1004</v>
+      </c>
+      <c r="J372" t="s">
+        <v>1012</v>
+      </c>
+      <c r="K372" s="2" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="373" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A373" s="34" t="s">
+        <v>855</v>
+      </c>
+      <c r="B373" s="32" t="s">
+        <v>855</v>
+      </c>
+      <c r="C373" s="3" t="s">
+        <v>986</v>
+      </c>
+      <c r="D373" s="2" t="s">
+        <v>994</v>
+      </c>
+      <c r="E373" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="H373" s="2">
+        <v>2</v>
+      </c>
+      <c r="I373" t="s">
+        <v>1005</v>
+      </c>
+      <c r="J373" t="s">
+        <v>1013</v>
+      </c>
+      <c r="K373" s="2" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="374" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A374" s="34" t="s">
+        <v>855</v>
+      </c>
+      <c r="B374" s="32" t="s">
+        <v>855</v>
+      </c>
+      <c r="C374" s="3" t="s">
+        <v>987</v>
+      </c>
+      <c r="D374" s="2" t="s">
+        <v>995</v>
+      </c>
+      <c r="E374" s="2" t="s">
+        <v>992</v>
+      </c>
+      <c r="H374" s="2">
+        <v>2</v>
+      </c>
+      <c r="I374" t="s">
+        <v>1006</v>
+      </c>
+      <c r="J374" t="s">
+        <v>1014</v>
+      </c>
+      <c r="K374" s="2" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="375" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A375" s="34" t="s">
+        <v>855</v>
+      </c>
+      <c r="B375" s="32" t="s">
+        <v>855</v>
+      </c>
+      <c r="C375" s="3" t="s">
+        <v>988</v>
+      </c>
+      <c r="D375" s="2" t="s">
+        <v>995</v>
+      </c>
+      <c r="E375" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="H375" s="2">
+        <v>2</v>
+      </c>
+      <c r="I375" t="s">
+        <v>1007</v>
+      </c>
+      <c r="J375" t="s">
+        <v>1015</v>
+      </c>
+      <c r="K375" s="2" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="376" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A376" s="34" t="s">
+        <v>855</v>
+      </c>
+      <c r="B376" s="32" t="s">
+        <v>855</v>
+      </c>
+      <c r="C376" s="3" t="s">
+        <v>989</v>
+      </c>
+      <c r="D376" s="2" t="s">
+        <v>995</v>
+      </c>
+      <c r="E376" s="2" t="s">
+        <v>992</v>
+      </c>
+      <c r="H376" s="2">
+        <v>2</v>
+      </c>
+      <c r="I376" t="s">
+        <v>1008</v>
+      </c>
+      <c r="J376" t="s">
+        <v>1014</v>
+      </c>
+      <c r="K376" s="2" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="377" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A377" s="34" t="s">
+        <v>855</v>
+      </c>
+      <c r="B377" s="32" t="s">
+        <v>855</v>
+      </c>
+      <c r="C377" s="3" t="s">
+        <v>990</v>
+      </c>
+      <c r="D377" s="2" t="s">
+        <v>995</v>
+      </c>
+      <c r="E377" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="H377" s="2">
+        <v>2</v>
+      </c>
+      <c r="I377" t="s">
+        <v>1009</v>
+      </c>
+      <c r="J377" t="s">
+        <v>1015</v>
+      </c>
+      <c r="K377" s="2" t="s">
+        <v>998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add functions for torque as f(power, rev)
Add functions for torque as f(power, rev). For English units, compute lbf-ft and lbf-inch as function of ft-lbf/sec and RPM and RPS. For SI units, compute newton-meter as function of watt and kilowatt. Update readme to reflect latest functionality.
</commit_message>
<xml_diff>
--- a/Reference/AeroToolKitFunctionList.xlsx
+++ b/Reference/AeroToolKitFunctionList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fs272\AeroProgs\StdAtmoAddIn\AeroToolKitAddIn\Reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85BD5A6-22D0-4BF7-B1A0-DC7042AF1405}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C9FB7C-0013-4298-845C-5AD3C40A16A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AeroToolKitFunctionList" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2882" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2966" uniqueCount="1043">
   <si>
     <t>KCAS</t>
   </si>
@@ -3033,9 +3033,6 @@
     <t>torqueLbfInch</t>
   </si>
   <si>
-    <t>newtonMeter</t>
-  </si>
-  <si>
     <t>lbf-ft/sec</t>
   </si>
   <si>
@@ -3045,39 +3042,6 @@
     <t>kilowatts</t>
   </si>
   <si>
-    <t>lbf-ft/sec, f(torque in lbf-ft, RPM)</t>
-  </si>
-  <si>
-    <t>lbf-ft/sec, f(torque in lbf-ft, RPS)</t>
-  </si>
-  <si>
-    <t>lbf-ft/sec, f(torque in lbf-inch, RPM)</t>
-  </si>
-  <si>
-    <t>lbf-ft/sec, f(torque in lbf-inch, RPS)</t>
-  </si>
-  <si>
-    <t>horsepower, f(torque in lbf-ft, RPS)</t>
-  </si>
-  <si>
-    <t>horsepower, f(torque in lbf-inch, RPM)</t>
-  </si>
-  <si>
-    <t>horsepower, f(torque in lbf-inch, RPS)</t>
-  </si>
-  <si>
-    <t>watts, f(torque in newton-meter, RPM)</t>
-  </si>
-  <si>
-    <t>watts, f(torque in newton-meter, RPS)</t>
-  </si>
-  <si>
-    <t>kilowatts, f(torque in newton-meter, RPM)</t>
-  </si>
-  <si>
-    <t>kilowatts, f(torque in newton-meter, RPS)</t>
-  </si>
-  <si>
     <t>lbf-ft, RPM</t>
   </si>
   <si>
@@ -3094,6 +3058,123 @@
   </si>
   <si>
     <t>newton-meter, RPS</t>
+  </si>
+  <si>
+    <t>AeroTorque_lbfFt_fPowerFtLbfPerSecRevPerMin</t>
+  </si>
+  <si>
+    <t>AeroTorque_lbfFt_fPowerFtLbfPerSecRevPerSec</t>
+  </si>
+  <si>
+    <t>AeroTorque_lbfFt_fPowerHorsepowerRevPerMin</t>
+  </si>
+  <si>
+    <t>AeroTorque_lbfFt_fPowerHorsepowerRevPerSec</t>
+  </si>
+  <si>
+    <t>AeroTorque_lbfInch_fPowerFtLbfPerSecRevPerMin</t>
+  </si>
+  <si>
+    <t>AeroTorque_lbfInch_fPowerFtLbfPerSecRevPerSec</t>
+  </si>
+  <si>
+    <t>AeroTorque_lbfInch_fPowerHorsepowerRevPerMin</t>
+  </si>
+  <si>
+    <t>AeroTorque_lbfInch_fPowerHorsepowerRevPerSec</t>
+  </si>
+  <si>
+    <t>AeroTorque_newtonMeter_fPowerKilowattsRevPerMin</t>
+  </si>
+  <si>
+    <t>AeroTorque_newtonMeter_fPowerKilowattsRevPerSec</t>
+  </si>
+  <si>
+    <t>AeroTorque_newtonMeter_fPowerWattsRevPerMin</t>
+  </si>
+  <si>
+    <t>AeroTorque_newtonMeter_fPowerWattsRevPerSec</t>
+  </si>
+  <si>
+    <t>torqueNewtonMeter</t>
+  </si>
+  <si>
+    <t>powerFtLbfPerSec</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> revPerMin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> revPerSec</t>
+  </si>
+  <si>
+    <t>powerHorsepower</t>
+  </si>
+  <si>
+    <t>powerKilowatts</t>
+  </si>
+  <si>
+    <t>powerWatts</t>
+  </si>
+  <si>
+    <t>lbf-ft/sec, RPM</t>
+  </si>
+  <si>
+    <t>lbf-ft/sec, RPS</t>
+  </si>
+  <si>
+    <t>horsepower, RPM</t>
+  </si>
+  <si>
+    <t>horsepower, RPS</t>
+  </si>
+  <si>
+    <t>watts, RPM</t>
+  </si>
+  <si>
+    <t>watts, RPS</t>
+  </si>
+  <si>
+    <t>kilowatts, RPM</t>
+  </si>
+  <si>
+    <t>kilowatts, RPS</t>
+  </si>
+  <si>
+    <t>Power in lbf-ft/sec, f(torque in lbf-ft, RPM)</t>
+  </si>
+  <si>
+    <t>Power in lbf-ft/sec, f(torque in lbf-ft, RPS)</t>
+  </si>
+  <si>
+    <t>Power in lbf-ft/sec, f(torque in lbf-inch, RPM)</t>
+  </si>
+  <si>
+    <t>Power in lbf-ft/sec, f(torque in lbf-inch, RPS)</t>
+  </si>
+  <si>
+    <t>Power in horsepower, f(torque in lbf-ft, RPM)</t>
+  </si>
+  <si>
+    <t>Power in horsepower, f(torque in lbf-ft, RPS)</t>
+  </si>
+  <si>
+    <t>Power in horsepower, f(torque in lbf-inch, RPM)</t>
+  </si>
+  <si>
+    <t>Power in horsepower, f(torque in lbf-inch, RPS)</t>
+  </si>
+  <si>
+    <t>Power in watts, f(torque in newton-meter, RPM)</t>
+  </si>
+  <si>
+    <t>Power in watts, f(torque in newton-meter, RPS)</t>
+  </si>
+  <si>
+    <t>Power in kilowatts, f(torque in newton-meter, RPM)</t>
+  </si>
+  <si>
+    <t>Power in kilowatts, f(torque in newton-meter, RPS)</t>
   </si>
 </sst>
 </file>
@@ -3143,7 +3224,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="29">
+  <fills count="30">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3311,6 +3392,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -3376,7 +3463,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -3786,7 +3873,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K377"/>
+  <dimension ref="A1:K389"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
@@ -3795,7 +3882,7 @@
     <col min="1" max="1" width="27.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -14000,13 +14087,13 @@
         <v>2</v>
       </c>
       <c r="I366" t="s">
-        <v>999</v>
+        <v>1031</v>
       </c>
       <c r="J366" t="s">
-        <v>1010</v>
+        <v>998</v>
       </c>
       <c r="K366" s="2" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="367" spans="1:11" x14ac:dyDescent="0.25">
@@ -14029,13 +14116,13 @@
         <v>2</v>
       </c>
       <c r="I367" t="s">
-        <v>1000</v>
+        <v>1032</v>
       </c>
       <c r="J367" t="s">
-        <v>1011</v>
+        <v>999</v>
       </c>
       <c r="K367" s="2" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="368" spans="1:11" x14ac:dyDescent="0.25">
@@ -14058,13 +14145,13 @@
         <v>2</v>
       </c>
       <c r="I368" t="s">
-        <v>1001</v>
+        <v>1033</v>
       </c>
       <c r="J368" t="s">
-        <v>1012</v>
+        <v>1000</v>
       </c>
       <c r="K368" s="2" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="369" spans="1:11" x14ac:dyDescent="0.25">
@@ -14087,13 +14174,13 @@
         <v>2</v>
       </c>
       <c r="I369" t="s">
-        <v>1002</v>
+        <v>1034</v>
       </c>
       <c r="J369" t="s">
-        <v>1013</v>
+        <v>1001</v>
       </c>
       <c r="K369" s="2" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="370" spans="1:11" x14ac:dyDescent="0.25">
@@ -14116,10 +14203,10 @@
         <v>2</v>
       </c>
       <c r="I370" t="s">
-        <v>999</v>
+        <v>1035</v>
       </c>
       <c r="J370" t="s">
-        <v>1010</v>
+        <v>998</v>
       </c>
       <c r="K370" s="2" t="s">
         <v>869</v>
@@ -14145,10 +14232,10 @@
         <v>2</v>
       </c>
       <c r="I371" t="s">
-        <v>1003</v>
+        <v>1036</v>
       </c>
       <c r="J371" t="s">
-        <v>1011</v>
+        <v>999</v>
       </c>
       <c r="K371" s="2" t="s">
         <v>869</v>
@@ -14174,10 +14261,10 @@
         <v>2</v>
       </c>
       <c r="I372" t="s">
-        <v>1004</v>
+        <v>1037</v>
       </c>
       <c r="J372" t="s">
-        <v>1012</v>
+        <v>1000</v>
       </c>
       <c r="K372" s="2" t="s">
         <v>869</v>
@@ -14203,10 +14290,10 @@
         <v>2</v>
       </c>
       <c r="I373" t="s">
-        <v>1005</v>
+        <v>1038</v>
       </c>
       <c r="J373" t="s">
-        <v>1013</v>
+        <v>1001</v>
       </c>
       <c r="K373" s="2" t="s">
         <v>869</v>
@@ -14223,7 +14310,7 @@
         <v>987</v>
       </c>
       <c r="D374" s="2" t="s">
-        <v>995</v>
+        <v>1016</v>
       </c>
       <c r="E374" s="2" t="s">
         <v>992</v>
@@ -14232,13 +14319,13 @@
         <v>2</v>
       </c>
       <c r="I374" t="s">
-        <v>1006</v>
+        <v>1039</v>
       </c>
       <c r="J374" t="s">
-        <v>1014</v>
+        <v>1002</v>
       </c>
       <c r="K374" s="2" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="375" spans="1:11" x14ac:dyDescent="0.25">
@@ -14252,7 +14339,7 @@
         <v>988</v>
       </c>
       <c r="D375" s="2" t="s">
-        <v>995</v>
+        <v>1016</v>
       </c>
       <c r="E375" s="2" t="s">
         <v>993</v>
@@ -14261,13 +14348,13 @@
         <v>2</v>
       </c>
       <c r="I375" t="s">
-        <v>1007</v>
+        <v>1040</v>
       </c>
       <c r="J375" t="s">
-        <v>1015</v>
+        <v>1003</v>
       </c>
       <c r="K375" s="2" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="376" spans="1:11" x14ac:dyDescent="0.25">
@@ -14281,7 +14368,7 @@
         <v>989</v>
       </c>
       <c r="D376" s="2" t="s">
-        <v>995</v>
+        <v>1016</v>
       </c>
       <c r="E376" s="2" t="s">
         <v>992</v>
@@ -14290,13 +14377,13 @@
         <v>2</v>
       </c>
       <c r="I376" t="s">
-        <v>1008</v>
+        <v>1041</v>
       </c>
       <c r="J376" t="s">
-        <v>1014</v>
+        <v>1002</v>
       </c>
       <c r="K376" s="2" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="377" spans="1:11" x14ac:dyDescent="0.25">
@@ -14310,7 +14397,7 @@
         <v>990</v>
       </c>
       <c r="D377" s="2" t="s">
-        <v>995</v>
+        <v>1016</v>
       </c>
       <c r="E377" s="2" t="s">
         <v>993</v>
@@ -14319,13 +14406,373 @@
         <v>2</v>
       </c>
       <c r="I377" t="s">
+        <v>1042</v>
+      </c>
+      <c r="J377" t="s">
+        <v>1003</v>
+      </c>
+      <c r="K377" s="2" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="378" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A378" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="B378" s="25" t="s">
+        <v>824</v>
+      </c>
+      <c r="C378" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D378" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E378" t="s">
+        <v>1018</v>
+      </c>
+      <c r="H378" s="2">
+        <v>2</v>
+      </c>
+      <c r="I378" s="2" t="str">
+        <f>"Torque in " &amp;K378&amp;", f("&amp;J378&amp;")"</f>
+        <v>Torque in lbf-ft, f(lbf-ft/sec, RPM)</v>
+      </c>
+      <c r="J378" t="s">
+        <v>1023</v>
+      </c>
+      <c r="K378" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A379" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="B379" s="25" t="s">
+        <v>824</v>
+      </c>
+      <c r="C379" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D379" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E379" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H379" s="2">
+        <v>2</v>
+      </c>
+      <c r="I379" s="2" t="str">
+        <f t="shared" ref="I379:I389" si="0">"Torque in " &amp;K379&amp;", f("&amp;J379&amp;")"</f>
+        <v>Torque in lbf-ft, f(lbf-ft/sec, RPS)</v>
+      </c>
+      <c r="J379" t="s">
+        <v>1024</v>
+      </c>
+      <c r="K379" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="380" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A380" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="B380" s="25" t="s">
+        <v>824</v>
+      </c>
+      <c r="C380" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D380" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E380" t="s">
+        <v>1018</v>
+      </c>
+      <c r="H380" s="2">
+        <v>2</v>
+      </c>
+      <c r="I380" s="2" t="str">
+        <f>"Torque in " &amp;K380&amp;", f("&amp;J380&amp;")"</f>
+        <v>Torque in lbf-ft, f(horsepower, RPM)</v>
+      </c>
+      <c r="J380" t="s">
+        <v>1025</v>
+      </c>
+      <c r="K380" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="381" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A381" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="B381" s="25" t="s">
+        <v>824</v>
+      </c>
+      <c r="C381" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D381" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E381" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H381" s="2">
+        <v>2</v>
+      </c>
+      <c r="I381" s="2" t="str">
+        <f>"Torque in " &amp;K381&amp;", f("&amp;J381&amp;")"</f>
+        <v>Torque in lbf-ft, f(horsepower, RPS)</v>
+      </c>
+      <c r="J381" t="s">
+        <v>1026</v>
+      </c>
+      <c r="K381" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="382" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A382" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="B382" s="25" t="s">
+        <v>824</v>
+      </c>
+      <c r="C382" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D382" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E382" t="s">
+        <v>1018</v>
+      </c>
+      <c r="H382" s="2">
+        <v>2</v>
+      </c>
+      <c r="I382" s="2" t="str">
+        <f>"Torque in " &amp;K382&amp;", f("&amp;J382&amp;")"</f>
+        <v>Torque in lbf-inch, f(lbf-ft/sec, RPM)</v>
+      </c>
+      <c r="J382" t="s">
+        <v>1023</v>
+      </c>
+      <c r="K382" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A383" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="B383" s="25" t="s">
+        <v>824</v>
+      </c>
+      <c r="C383" t="s">
         <v>1009</v>
       </c>
-      <c r="J377" t="s">
+      <c r="D383" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E383" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H383" s="2">
+        <v>2</v>
+      </c>
+      <c r="I383" s="2" t="str">
+        <f>"Torque in " &amp;K383&amp;", f("&amp;J383&amp;")"</f>
+        <v>Torque in lbf-inch, f(lbf-ft/sec, RPS)</v>
+      </c>
+      <c r="J383" t="s">
+        <v>1024</v>
+      </c>
+      <c r="K383" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A384" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="B384" s="25" t="s">
+        <v>824</v>
+      </c>
+      <c r="C384" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D384" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E384" t="s">
+        <v>1018</v>
+      </c>
+      <c r="H384" s="2">
+        <v>2</v>
+      </c>
+      <c r="I384" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Torque in lbf-inch, f(horsepower, RPM)</v>
+      </c>
+      <c r="J384" t="s">
+        <v>1025</v>
+      </c>
+      <c r="K384" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A385" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="B385" s="25" t="s">
+        <v>824</v>
+      </c>
+      <c r="C385" t="s">
+        <v>1011</v>
+      </c>
+      <c r="D385" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E385" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H385" s="2">
+        <v>2</v>
+      </c>
+      <c r="I385" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Torque in lbf-inch, f(horsepower, RPS)</v>
+      </c>
+      <c r="J385" t="s">
+        <v>1026</v>
+      </c>
+      <c r="K385" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A386" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="B386" s="25" t="s">
+        <v>824</v>
+      </c>
+      <c r="C386" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D386" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E386" t="s">
+        <v>1018</v>
+      </c>
+      <c r="H386" s="2">
+        <v>2</v>
+      </c>
+      <c r="I386" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Torque in newton-meter, f(watts, RPM)</v>
+      </c>
+      <c r="J386" t="s">
+        <v>1027</v>
+      </c>
+      <c r="K386" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A387" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="B387" s="25" t="s">
+        <v>824</v>
+      </c>
+      <c r="C387" t="s">
         <v>1015</v>
       </c>
-      <c r="K377" s="2" t="s">
-        <v>998</v>
+      <c r="D387" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E387" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H387" s="2">
+        <v>2</v>
+      </c>
+      <c r="I387" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Torque in newton-meter, f(watts, RPS)</v>
+      </c>
+      <c r="J387" t="s">
+        <v>1028</v>
+      </c>
+      <c r="K387" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A388" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="B388" s="25" t="s">
+        <v>824</v>
+      </c>
+      <c r="C388" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D388" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E388" t="s">
+        <v>1018</v>
+      </c>
+      <c r="H388" s="2">
+        <v>2</v>
+      </c>
+      <c r="I388" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Torque in newton-meter, f(kilowatts, RPM)</v>
+      </c>
+      <c r="J388" t="s">
+        <v>1029</v>
+      </c>
+      <c r="K388" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A389" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="B389" s="25" t="s">
+        <v>824</v>
+      </c>
+      <c r="C389" t="s">
+        <v>1013</v>
+      </c>
+      <c r="D389" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E389" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H389" s="2">
+        <v>2</v>
+      </c>
+      <c r="I389" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Torque in newton-meter, f(kilowatts, RPS)</v>
+      </c>
+      <c r="J389" t="s">
+        <v>1030</v>
+      </c>
+      <c r="K389" t="s">
+        <v>853</v>
       </c>
     </row>
   </sheetData>

</xml_diff>